<commit_message>
updated MotorPot firmware and BOMs
</commit_message>
<xml_diff>
--- a/Eurorack_MotorPot/Eurorack_MotorPot_bom.xlsx
+++ b/Eurorack_MotorPot/Eurorack_MotorPot_bom.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Documents/GitHub/Midi-boards/Eurorack_MotorPot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320B2077-BCF8-0A46-824D-4AE9BDB27B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5D7DA5-6788-E841-BFEB-10A7836B642F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47040" yWindow="880" windowWidth="19760" windowHeight="20980" xr2:uid="{B1A2F949-7E6C-8644-8E19-B56F3D22CDD7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{B1A2F949-7E6C-8644-8E19-B56F3D22CDD7}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorPot" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">MotorPot!$A$1:$E$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">MotorPot!$A$1:$E$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -671,7 +671,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -718,14 +718,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -735,6 +727,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -760,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -891,12 +899,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -905,58 +935,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,10 +1366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AJ119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="104" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="104" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1400,13 +1430,13 @@
       </c>
     </row>
     <row r="2" spans="1:36" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
       <c r="AF2">
         <v>17</v>
       </c>
@@ -1424,11 +1454,11 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
@@ -1523,35 +1553,35 @@
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="14" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="14" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <v>1</v>
       </c>
       <c r="AF10">
@@ -1612,30 +1642,30 @@
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="10">
         <v>1</v>
       </c>
       <c r="AF14">
@@ -1655,32 +1685,32 @@
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="11" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1726,17 +1756,17 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="14">
         <v>104</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="9">
         <v>1</v>
       </c>
       <c r="AF19">
@@ -1756,32 +1786,32 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="11" t="s">
         <v>131</v>
       </c>
       <c r="AF21">
@@ -1801,17 +1831,17 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="9">
         <v>1</v>
       </c>
       <c r="AF22">
@@ -1831,11 +1861,6 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
       <c r="AF23">
         <v>24</v>
       </c>
@@ -1876,132 +1901,127 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14" t="s">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14" t="s">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E26" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14" t="s">
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E28" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14" t="s">
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14" t="s">
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E30" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14" t="s">
+      <c r="E30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E31" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:36" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14" t="s">
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
       <c r="AF33">
         <v>24</v>
       </c>
@@ -2043,71 +2063,66 @@
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
       <c r="AF39">
         <v>25</v>
       </c>
@@ -2149,77 +2164,77 @@
       </c>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="9">
         <v>4</v>
       </c>
       <c r="AF45">
@@ -2239,17 +2254,17 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="9">
         <v>5</v>
       </c>
       <c r="AF46">
@@ -2269,180 +2284,180 @@
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15" t="s">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15">
+      <c r="D55" s="9"/>
+      <c r="E55" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18" t="s">
+      <c r="A56" s="9"/>
+      <c r="B56" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E56" s="18">
+      <c r="E56" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="9">
         <v>4</v>
       </c>
       <c r="AF58">
@@ -2462,18 +2477,13 @@
       </c>
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
       <c r="AF60">
         <v>32</v>
       </c>
@@ -2494,10 +2504,10 @@
       <c r="A61" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="24"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="16"/>
       <c r="AF61">
         <v>33</v>
       </c>
@@ -2515,11 +2525,11 @@
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A62" s="25"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
-      <c r="E62" s="26"/>
+      <c r="E62" s="21"/>
     </row>
     <row r="63" spans="1:36" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
@@ -2527,8 +2537,7 @@
       </c>
       <c r="B63" s="28"/>
       <c r="C63" s="28"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="26"/>
+      <c r="E63" s="18"/>
       <c r="AF63">
         <v>34</v>
       </c>
@@ -2546,13 +2555,10 @@
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
+      <c r="E64" s="18"/>
     </row>
     <row r="65" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
@@ -2608,8 +2614,7 @@
       </c>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="26"/>
+      <c r="E67" s="18"/>
       <c r="AF67">
         <v>37</v>
       </c>
@@ -2627,13 +2632,12 @@
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="26"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="E68" s="18"/>
       <c r="AF68">
         <v>38</v>
       </c>
@@ -3527,20 +3531,20 @@
     <sortCondition ref="A1:A120"/>
   </sortState>
   <mergeCells count="7">
+    <mergeCell ref="A68:C68"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A66:E66"/>
     <mergeCell ref="A67:C67"/>
     <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A68:C68"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{74E1F473-C408-FF48-A715-37A536DE1EC7}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="60" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="57" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="10"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>